<commit_message>
create model for only appendEvent actions
</commit_message>
<xml_diff>
--- a/test/resources/Simulant.xlsx
+++ b/test/resources/Simulant.xlsx
@@ -489,7 +489,7 @@
   <dimension ref="A1:C2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -516,7 +516,7 @@
         <v>9</v>
       </c>
       <c r="C2">
-        <f>SUM(EventLog!B2:B31)</f>
+        <f>SUM(EventLog!B2:B1000)</f>
         <v>0</v>
       </c>
     </row>

</xml_diff>